<commit_message>
update .xlsx and .md
</commit_message>
<xml_diff>
--- a/3-Testing_Documentation_&_Test_Case/Praktikum/Muhamad_Nur_Fajjri_Z_TEST_CASE.xlsx
+++ b/3-Testing_Documentation_&_Test_Case/Praktikum/Muhamad_Nur_Fajjri_Z_TEST_CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.MATERI KULIAH\SEMESTER-8_QE_ALTERRA\QE_Muhamad-Nur-Fajjri-Z\3-Testing_Documentation_&amp;_Test_Case\Praktikum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8E00E7-5775-4D6B-9205-5AA82256660C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B2DF44-1602-4A0B-82FB-4D573A15E94C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1E79758F-6DCE-4028-A25E-D68964AEB67C}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -195,6 +195,24 @@
   </si>
   <si>
     <t>TIDAK_DIEKSEKUSI</t>
+  </si>
+  <si>
+    <t>Pengguna memilih opsi pada halaman utama sepulsa.com (pulsa, voucher game, listrik PLN, dkk</t>
+  </si>
+  <si>
+    <t>ospi terpilih dan masuk ke menu selanjutnya</t>
+  </si>
+  <si>
+    <t>pengguna mengisi form control pada salah satu opsi (kasus contoh pulsa)</t>
+  </si>
+  <si>
+    <t>form terisi dan transaksi di proses</t>
+  </si>
+  <si>
+    <t>pengguna tidak mengisi form control pada salah satu opsi</t>
+  </si>
+  <si>
+    <t>transaksi tidak berjalan</t>
   </si>
 </sst>
 </file>
@@ -477,7 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -537,6 +555,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -557,8 +578,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -618,6 +640,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -724,9 +749,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C36661-0104-44D0-8912-6232ACE965BE}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1057,56 +1079,56 @@
     <col min="6" max="7" width="9.140625" style="2"/>
     <col min="8" max="9" width="12.42578125" style="2" customWidth="1"/>
     <col min="10" max="12" width="9.140625" style="2"/>
-    <col min="13" max="13" width="3.42578125" style="86" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" style="21" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="36" t="s">
+      <c r="G2" s="38"/>
+      <c r="H2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="37" t="s">
+      <c r="I2" s="36"/>
+      <c r="J2" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="38"/>
+      <c r="K2" s="42"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -1122,10 +1144,10 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="20" t="s">
         <v>7</v>
       </c>
@@ -1152,33 +1174,33 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="40"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="41">
+      <c r="E6" s="44"/>
+      <c r="F6" s="45">
         <v>44983</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="43" t="s">
+      <c r="G6" s="46"/>
+      <c r="H6" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="29" t="s">
+      <c r="I6" s="48"/>
+      <c r="J6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="30"/>
-      <c r="M6" s="87" t="s">
+      <c r="K6" s="34"/>
+      <c r="M6" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="N6" s="88" t="s">
+      <c r="N6" s="23" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1194,10 +1216,10 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="M7" s="87">
+      <c r="M7" s="22">
         <v>1</v>
       </c>
-      <c r="N7" s="88" t="s">
+      <c r="N7" s="23" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1205,26 +1227,26 @@
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="7"/>
       <c r="F8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="M8" s="87">
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="M8" s="22">
         <v>2</v>
       </c>
-      <c r="N8" s="88" t="s">
+      <c r="N8" s="23" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1232,26 +1254,26 @@
       <c r="A9" s="9">
         <v>1</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="3"/>
       <c r="F9" s="9">
         <v>1</v>
       </c>
-      <c r="G9" s="48" t="s">
+      <c r="G9" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="34"/>
-      <c r="M9" s="87">
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="38"/>
+      <c r="M9" s="22">
         <v>3</v>
       </c>
-      <c r="N9" s="88" t="s">
+      <c r="N9" s="23" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1259,24 +1281,24 @@
       <c r="A10" s="9">
         <v>2</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="3"/>
       <c r="F10" s="9">
         <v>2</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="34"/>
-      <c r="M10" s="87">
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="38"/>
+      <c r="M10" s="22">
         <v>4</v>
       </c>
-      <c r="N10" s="88" t="s">
+      <c r="N10" s="23" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1284,35 +1306,35 @@
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="3"/>
       <c r="F11" s="9">
         <v>3</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="34"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="38"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>4</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="3"/>
       <c r="F12" s="9">
         <v>4</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="34"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="38"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -1345,224 +1367,224 @@
       <c r="K14" s="3"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="22" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="22" t="s">
+      <c r="E16" s="26"/>
+      <c r="F16" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="22" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>1</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="21" t="s">
+      <c r="C18" s="53"/>
+      <c r="D18" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21" t="s">
+      <c r="E18" s="24"/>
+      <c r="F18" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21" t="s">
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>2</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="21" t="s">
+      <c r="C19" s="30"/>
+      <c r="D19" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21" t="s">
+      <c r="E19" s="24"/>
+      <c r="F19" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21" t="s">
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>3</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="21" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21" t="s">
+      <c r="E20" s="24"/>
+      <c r="F20" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21" t="s">
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>4</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="21" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21" t="s">
+      <c r="E21" s="24"/>
+      <c r="F21" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21" t="s">
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
         <v>5</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="21" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21" t="s">
+      <c r="E22" s="24"/>
+      <c r="F22" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21" t="s">
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>6</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="21" t="s">
+      <c r="C23" s="30"/>
+      <c r="D23" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21" t="s">
+      <c r="E23" s="24"/>
+      <c r="F23" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21" t="s">
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>7</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="21" t="s">
+      <c r="C24" s="30"/>
+      <c r="D24" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21" t="s">
+      <c r="E24" s="24"/>
+      <c r="F24" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21" t="s">
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>8</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="21" t="s">
+      <c r="C25" s="30"/>
+      <c r="D25" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21" t="s">
+      <c r="E25" s="24"/>
+      <c r="F25" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21" t="s">
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
@@ -1582,160 +1604,184 @@
       <c r="K27" s="3"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="22" t="s">
+      <c r="C29" s="26"/>
+      <c r="D29" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="22" t="s">
+      <c r="E29" s="26"/>
+      <c r="F29" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="22" t="s">
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>1</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+    </row>
+    <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
         <v>2</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
+      <c r="B32" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>3</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
+      <c r="B33" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>4</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>5</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
         <v>6</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>7</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
         <v>8</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="98">
@@ -1838,9 +1884,6 @@
     <mergeCell ref="F38:H38"/>
     <mergeCell ref="I38:K38"/>
   </mergeCells>
-  <dataValidations xWindow="750" yWindow="427" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID_DATA" error="DATA SALAH" promptTitle="LOLOS" prompt="LOLOS" sqref="I18:K18" xr:uid="{54BF8AAA-E999-4B4A-8E98-BDADDE3486C2}"/>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1857,40 +1900,40 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="11"/>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="53"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="58"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="51"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="11"/>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="54" t="s">
+      <c r="E2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="61"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
@@ -1906,10 +1949,10 @@
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="58"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
@@ -1934,23 +1977,23 @@
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="60"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="14"/>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="59" t="s">
+      <c r="E6" s="65"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="60"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
@@ -1969,90 +2012,90 @@
       <c r="A8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
       <c r="E8" s="16"/>
       <c r="F8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="50" t="s">
+      <c r="G8" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="66"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="71"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>1</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="53"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="12"/>
       <c r="F9" s="18">
         <v>1</v>
       </c>
-      <c r="G9" s="67"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="53"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="58"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>2</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="53"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="58"/>
       <c r="E10" s="12"/>
       <c r="F10" s="18">
         <v>2</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="53"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="58"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>3</v>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="53"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="58"/>
       <c r="E11" s="12"/>
       <c r="F11" s="18">
         <v>3</v>
       </c>
-      <c r="G11" s="67"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="53"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>4</v>
       </c>
-      <c r="B12" s="67"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="53"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="58"/>
       <c r="E12" s="12"/>
       <c r="F12" s="18">
         <v>4</v>
       </c>
-      <c r="G12" s="67"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="53"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="58"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
@@ -2083,118 +2126,118 @@
       <c r="K14" s="12"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="74" t="s">
+      <c r="C16" s="76"/>
+      <c r="D16" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="75"/>
-      <c r="F16" s="70" t="s">
+      <c r="E16" s="80"/>
+      <c r="F16" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="78"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="70" t="s">
+      <c r="G16" s="83"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="78"/>
-      <c r="K16" s="79"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="84"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="82"/>
+      <c r="A17" s="74"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="87"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="53"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="58"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="53"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="58"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="53"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="58"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="53"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="58"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="53"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="58"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="53"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="53">
@@ -2267,40 +2310,40 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="11"/>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="53"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="58"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="51"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="11"/>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="54" t="s">
+      <c r="E2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="61"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
@@ -2316,10 +2359,10 @@
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="58"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
@@ -2344,23 +2387,23 @@
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="60"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="14"/>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="84" t="s">
+      <c r="E6" s="65"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="85"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
@@ -2379,90 +2422,90 @@
       <c r="A8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
       <c r="E8" s="16"/>
       <c r="F8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="50" t="s">
+      <c r="G8" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="66"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="71"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>1</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="53"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="12"/>
       <c r="F9" s="18">
         <v>1</v>
       </c>
-      <c r="G9" s="67"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="53"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="58"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>2</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="53"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="58"/>
       <c r="E10" s="12"/>
       <c r="F10" s="18">
         <v>2</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="53"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="58"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>3</v>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="53"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="58"/>
       <c r="E11" s="12"/>
       <c r="F11" s="18">
         <v>3</v>
       </c>
-      <c r="G11" s="67"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="53"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>4</v>
       </c>
-      <c r="B12" s="67"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="53"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="58"/>
       <c r="E12" s="12"/>
       <c r="F12" s="18">
         <v>4</v>
       </c>
-      <c r="G12" s="67"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="53"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="58"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
@@ -2493,118 +2536,118 @@
       <c r="K14" s="12"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="74" t="s">
+      <c r="C16" s="76"/>
+      <c r="D16" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="75"/>
-      <c r="F16" s="70" t="s">
+      <c r="E16" s="80"/>
+      <c r="F16" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="78"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="70" t="s">
+      <c r="G16" s="83"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="78"/>
-      <c r="K16" s="79"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="84"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="82"/>
+      <c r="A17" s="74"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="87"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="53"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="58"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="53"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="58"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="53"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="58"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="53"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="58"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="53"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="58"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="53"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="53">

</xml_diff>